<commit_message>
Entry NC: Added CDD Instruction Sheet for USD and YEN for Return to JS Payroll
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_NC_RET_USD.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/CDDIS_NC_RET_USD.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Apprv.</t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>.</t>
   </si>
 </sst>
 </file>
@@ -760,9 +757,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -839,12 +833,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -871,18 +859,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,29 +906,11 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -966,15 +924,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -989,73 +938,121 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1437,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AT9" sqref="AT9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="AR29" sqref="AR29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1645,27 +1642,27 @@
       </c>
       <c r="T5" s="21"/>
       <c r="U5" s="22"/>
-      <c r="V5" s="23">
+      <c r="V5" s="127">
         <f ca="1">NOW()</f>
-        <v>43676.598017939818</v>
-      </c>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
+        <v>43676.720926620372</v>
+      </c>
+      <c r="W5" s="127"/>
+      <c r="X5" s="127"/>
+      <c r="Y5" s="127"/>
+      <c r="Z5" s="127"/>
+      <c r="AA5" s="127"/>
+      <c r="AB5" s="127"/>
       <c r="AC5" s="6"/>
       <c r="AD5" s="6"/>
       <c r="AE5" s="6"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="25"/>
-      <c r="AH5" s="25"/>
-      <c r="AI5" s="26"/>
-      <c r="AJ5" s="25"/>
-      <c r="AK5" s="25"/>
-      <c r="AL5" s="25"/>
-      <c r="AM5" s="26"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="25"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
+      <c r="AL5" s="24"/>
+      <c r="AM5" s="25"/>
       <c r="AN5" s="10"/>
     </row>
     <row r="6" spans="1:40" ht="9" customHeight="1" x14ac:dyDescent="0.25">
@@ -1687,7 +1684,7 @@
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
-      <c r="S6" s="27"/>
+      <c r="S6" s="26"/>
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
       <c r="V6" s="13"/>
@@ -1711,7 +1708,7 @@
       <c r="AN6" s="10"/>
     </row>
     <row r="7" spans="1:40" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1729,7 +1726,7 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
-      <c r="S7" s="27"/>
+      <c r="S7" s="26"/>
       <c r="T7" s="13"/>
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
@@ -1753,710 +1750,693 @@
       <c r="AN7" s="10"/>
     </row>
     <row r="8" spans="1:40" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32">
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="31">
         <v>0</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>5</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="35">
+      <c r="G8" s="33"/>
+      <c r="H8" s="34">
         <v>2</v>
       </c>
-      <c r="I8" s="33">
+      <c r="I8" s="32">
         <v>4</v>
       </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35">
+      <c r="J8" s="33"/>
+      <c r="K8" s="34">
         <v>1</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="32">
         <v>9</v>
       </c>
       <c r="M8" s="6"/>
-      <c r="N8" s="30" t="s">
+      <c r="N8" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="30"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
       <c r="S8" s="6"/>
-      <c r="T8" s="36" t="s">
+      <c r="T8" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="U8" s="37" t="s">
+      <c r="U8" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="V8" s="38"/>
-      <c r="W8" s="34" t="s">
+      <c r="V8" s="37"/>
+      <c r="W8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="X8" s="36">
+      <c r="X8" s="35">
         <v>7</v>
       </c>
-      <c r="Y8" s="37">
+      <c r="Y8" s="36">
         <v>8</v>
       </c>
-      <c r="Z8" s="39">
+      <c r="Z8" s="38">
         <v>9</v>
       </c>
-      <c r="AA8" s="34" t="s">
+      <c r="AA8" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="AB8" s="40"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="41"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
-      <c r="AG8" s="38"/>
-      <c r="AH8" s="30" t="s">
+      <c r="AB8" s="39"/>
+      <c r="AC8" s="40"/>
+      <c r="AD8" s="40"/>
+      <c r="AE8" s="40"/>
+      <c r="AF8" s="40"/>
+      <c r="AG8" s="37"/>
+      <c r="AH8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="AI8" s="30"/>
-      <c r="AJ8" s="30"/>
+      <c r="AI8" s="29"/>
+      <c r="AJ8" s="29"/>
       <c r="AK8" s="6"/>
-      <c r="AL8" s="42"/>
-      <c r="AM8" s="42"/>
-      <c r="AN8" s="43"/>
+      <c r="AL8" s="41"/>
+      <c r="AM8" s="41"/>
+      <c r="AN8" s="42"/>
     </row>
     <row r="9" spans="1:40" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="44">
+      <c r="B9" s="29"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="43">
         <v>0</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="44">
         <v>9</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="30"/>
+      <c r="H9" s="29"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="46"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="47"/>
-      <c r="Q9" s="47"/>
-      <c r="R9" s="47"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="47"/>
-      <c r="AB9" s="47"/>
-      <c r="AC9" s="47"/>
-      <c r="AD9" s="47"/>
-      <c r="AE9" s="47"/>
-      <c r="AF9" s="47"/>
-      <c r="AG9" s="47"/>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
-      <c r="AK9" s="47"/>
-      <c r="AL9" s="47"/>
-      <c r="AM9" s="47"/>
-      <c r="AN9" s="49"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="46"/>
+      <c r="Y9" s="46"/>
+      <c r="Z9" s="46"/>
+      <c r="AA9" s="46"/>
+      <c r="AB9" s="46"/>
+      <c r="AC9" s="46"/>
+      <c r="AD9" s="46"/>
+      <c r="AE9" s="46"/>
+      <c r="AF9" s="46"/>
+      <c r="AG9" s="46"/>
+      <c r="AH9" s="46"/>
+      <c r="AI9" s="46"/>
+      <c r="AJ9" s="46"/>
+      <c r="AK9" s="46"/>
+      <c r="AL9" s="46"/>
+      <c r="AM9" s="46"/>
+      <c r="AN9" s="48"/>
     </row>
     <row r="10" spans="1:40" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="51"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="30"/>
-      <c r="X10" s="30"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="29"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="29"/>
+      <c r="Y10" s="29"/>
+      <c r="Z10" s="29"/>
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
       <c r="AD10" s="6"/>
-      <c r="AE10" s="30"/>
+      <c r="AE10" s="29"/>
       <c r="AF10" s="6"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
-      <c r="AJ10" s="52" t="s">
+      <c r="AJ10" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="AK10" s="53"/>
-      <c r="AL10" s="53"/>
-      <c r="AM10" s="54"/>
-      <c r="AN10" s="43"/>
+      <c r="AK10" s="113"/>
+      <c r="AL10" s="113"/>
+      <c r="AM10" s="51"/>
+      <c r="AN10" s="42"/>
     </row>
     <row r="11" spans="1:40" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="30"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
-      <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="30"/>
-      <c r="X11" s="30"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="29"/>
+      <c r="U11" s="29"/>
+      <c r="V11" s="29"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="29"/>
+      <c r="Y11" s="29"/>
+      <c r="Z11" s="29"/>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
       <c r="AD11" s="6"/>
-      <c r="AE11" s="30"/>
+      <c r="AE11" s="29"/>
       <c r="AF11" s="6"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
-      <c r="AJ11" s="56"/>
-      <c r="AK11" s="30"/>
-      <c r="AL11" s="30"/>
+      <c r="AJ11" s="53"/>
+      <c r="AK11" s="29"/>
+      <c r="AL11" s="29"/>
       <c r="AM11" s="6"/>
-      <c r="AN11" s="43"/>
+      <c r="AN11" s="42"/>
     </row>
     <row r="12" spans="1:40" ht="3.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="59"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="59"/>
-      <c r="U12" s="59"/>
-      <c r="V12" s="59"/>
-      <c r="W12" s="59"/>
-      <c r="X12" s="59"/>
-      <c r="Y12" s="59"/>
-      <c r="Z12" s="59"/>
-      <c r="AA12" s="60"/>
-      <c r="AB12" s="60"/>
-      <c r="AC12" s="60"/>
-      <c r="AD12" s="60"/>
-      <c r="AE12" s="59"/>
-      <c r="AF12" s="60"/>
-      <c r="AG12" s="60"/>
-      <c r="AH12" s="60"/>
-      <c r="AI12" s="60"/>
-      <c r="AJ12" s="61"/>
-      <c r="AK12" s="59"/>
-      <c r="AL12" s="59"/>
-      <c r="AM12" s="60"/>
-      <c r="AN12" s="62"/>
+      <c r="A12" s="54"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="56"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="56"/>
+      <c r="V12" s="56"/>
+      <c r="W12" s="56"/>
+      <c r="X12" s="56"/>
+      <c r="Y12" s="56"/>
+      <c r="Z12" s="56"/>
+      <c r="AA12" s="57"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="56"/>
+      <c r="AF12" s="57"/>
+      <c r="AG12" s="57"/>
+      <c r="AH12" s="57"/>
+      <c r="AI12" s="57"/>
+      <c r="AJ12" s="58"/>
+      <c r="AK12" s="56"/>
+      <c r="AL12" s="56"/>
+      <c r="AM12" s="57"/>
+      <c r="AN12" s="59"/>
     </row>
     <row r="13" spans="1:40" ht="3" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="30">
+      <c r="A13" s="60"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+      <c r="T13" s="29"/>
+      <c r="U13" s="29"/>
+      <c r="V13" s="29"/>
+      <c r="W13" s="29"/>
+      <c r="X13" s="29">
         <v>6</v>
       </c>
-      <c r="Y13" s="30">
+      <c r="Y13" s="29">
         <v>0</v>
       </c>
-      <c r="Z13" s="30">
+      <c r="Z13" s="29">
         <v>0</v>
       </c>
-      <c r="AA13" s="30"/>
-      <c r="AB13" s="30"/>
-      <c r="AC13" s="30"/>
-      <c r="AD13" s="30"/>
-      <c r="AE13" s="30"/>
-      <c r="AF13" s="30"/>
-      <c r="AG13" s="30"/>
-      <c r="AH13" s="30"/>
-      <c r="AI13" s="30"/>
-      <c r="AJ13" s="30"/>
-      <c r="AK13" s="30"/>
-      <c r="AL13" s="30"/>
-      <c r="AM13" s="30"/>
-      <c r="AN13" s="43"/>
+      <c r="AA13" s="29"/>
+      <c r="AB13" s="29"/>
+      <c r="AC13" s="29"/>
+      <c r="AD13" s="29"/>
+      <c r="AE13" s="29"/>
+      <c r="AF13" s="29"/>
+      <c r="AG13" s="29"/>
+      <c r="AH13" s="29"/>
+      <c r="AI13" s="29"/>
+      <c r="AJ13" s="29"/>
+      <c r="AK13" s="29"/>
+      <c r="AL13" s="29"/>
+      <c r="AM13" s="29"/>
+      <c r="AN13" s="42"/>
     </row>
     <row r="14" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66" t="s">
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="128"/>
+      <c r="E14" s="125" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="30"/>
-      <c r="I14" s="30" t="s">
+      <c r="F14" s="129"/>
+      <c r="G14" s="29"/>
+      <c r="I14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="68" t="s">
+      <c r="M14" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="N14" s="69" t="s">
+      <c r="N14" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="O14" s="69" t="s">
+      <c r="O14" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="70"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30" t="s">
+      <c r="P14" s="63"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="T14" s="71"/>
-      <c r="U14" s="71"/>
-      <c r="V14" s="71"/>
-      <c r="W14" s="72"/>
-      <c r="X14" s="73">
-        <f>X24</f>
-        <v>7</v>
-      </c>
-      <c r="Y14" s="73">
-        <f>Y24</f>
-        <v>3</v>
-      </c>
-      <c r="Z14" s="73">
-        <f>Z24</f>
-        <v>5</v>
-      </c>
-      <c r="AA14" s="73" t="str">
-        <f>AA24</f>
-        <v>.</v>
-      </c>
-      <c r="AB14" s="73">
-        <f>AB24</f>
+      <c r="T14" s="64"/>
+      <c r="U14" s="64"/>
+      <c r="V14" s="64"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="66"/>
+      <c r="Y14" s="66"/>
+      <c r="Z14" s="66"/>
+      <c r="AA14" s="66"/>
+      <c r="AB14" s="66"/>
+      <c r="AC14" s="66"/>
+      <c r="AD14" s="66"/>
+      <c r="AE14" s="67"/>
+      <c r="AF14" s="68"/>
+      <c r="AG14" s="68"/>
+      <c r="AH14" s="68"/>
+      <c r="AI14" s="68"/>
+      <c r="AJ14" s="68"/>
+      <c r="AK14" s="68"/>
+      <c r="AL14" s="68"/>
+      <c r="AM14" s="69"/>
+      <c r="AN14" s="10"/>
+    </row>
+    <row r="15" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="111" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="112"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="128"/>
+      <c r="E15" s="34">
+        <v>9</v>
+      </c>
+      <c r="F15" s="70">
         <v>0</v>
       </c>
-      <c r="AC14" s="73">
+      <c r="G15" s="70">
         <v>0</v>
       </c>
-      <c r="AD14" s="73"/>
-      <c r="AE14" s="74"/>
-      <c r="AF14" s="75"/>
-      <c r="AG14" s="75"/>
-      <c r="AH14" s="75"/>
-      <c r="AI14" s="75"/>
-      <c r="AJ14" s="75"/>
-      <c r="AK14" s="75"/>
-      <c r="AL14" s="75"/>
-      <c r="AM14" s="76"/>
-      <c r="AN14" s="10"/>
-    </row>
-    <row r="15" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="35">
-        <v>9</v>
-      </c>
-      <c r="F15" s="77">
-        <v>0</v>
-      </c>
-      <c r="G15" s="77">
-        <v>0</v>
-      </c>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="78"/>
-      <c r="K15" s="78"/>
-      <c r="L15" s="78"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="78"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="80"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
-      <c r="AB15" s="30"/>
-      <c r="AC15" s="30"/>
-      <c r="AD15" s="30"/>
-      <c r="AE15" s="30"/>
-      <c r="AF15" s="30"/>
-      <c r="AG15" s="30"/>
-      <c r="AH15" s="30"/>
-      <c r="AI15" s="30"/>
-      <c r="AJ15" s="30"/>
-      <c r="AK15" s="30"/>
-      <c r="AL15" s="30"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="70"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="71"/>
+      <c r="N15" s="71"/>
+      <c r="O15" s="71"/>
+      <c r="P15" s="72"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="64"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="29"/>
+      <c r="AB15" s="29"/>
+      <c r="AC15" s="29"/>
+      <c r="AD15" s="29"/>
+      <c r="AE15" s="29"/>
+      <c r="AF15" s="29"/>
+      <c r="AG15" s="29"/>
+      <c r="AH15" s="29"/>
+      <c r="AI15" s="29"/>
+      <c r="AJ15" s="29"/>
+      <c r="AK15" s="29"/>
+      <c r="AL15" s="29"/>
       <c r="AM15" s="6"/>
       <c r="AN15" s="10"/>
     </row>
     <row r="16" spans="1:40" s="12" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="81">
+      <c r="B16" s="112"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="128"/>
+      <c r="E16" s="74">
         <v>0</v>
       </c>
-      <c r="F16" s="82">
+      <c r="F16" s="75">
         <v>0</v>
       </c>
-      <c r="G16" s="82">
+      <c r="G16" s="75">
         <v>2</v>
       </c>
-      <c r="H16" s="82">
+      <c r="H16" s="75">
         <v>0</v>
       </c>
-      <c r="I16" s="83">
+      <c r="I16" s="76">
         <v>4</v>
       </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="30"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="30" t="s">
+      <c r="S16" s="29" t="s">
         <v>15</v>
       </c>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-      <c r="W16" s="30"/>
-      <c r="X16" s="30"/>
-      <c r="Y16" s="30"/>
-      <c r="Z16" s="36" t="s">
+      <c r="W16" s="29"/>
+      <c r="X16" s="29"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="AA16" s="37">
+      <c r="AA16" s="36">
         <v>7</v>
       </c>
-      <c r="AB16" s="39">
+      <c r="AB16" s="38">
         <v>9</v>
       </c>
-      <c r="AC16" s="84" t="s">
+      <c r="AC16" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="AD16" s="36">
+      <c r="AD16" s="35">
         <v>7</v>
       </c>
-      <c r="AE16" s="37">
+      <c r="AE16" s="36">
         <v>8</v>
       </c>
-      <c r="AF16" s="39">
+      <c r="AF16" s="38">
         <v>9</v>
       </c>
-      <c r="AG16" s="84" t="s">
+      <c r="AG16" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="AH16" s="36">
+      <c r="AH16" s="35">
         <v>1</v>
       </c>
-      <c r="AI16" s="37">
+      <c r="AI16" s="36">
         <v>5</v>
       </c>
-      <c r="AJ16" s="37">
+      <c r="AJ16" s="36">
         <v>1</v>
       </c>
-      <c r="AK16" s="37">
+      <c r="AK16" s="36">
         <v>1</v>
       </c>
-      <c r="AL16" s="37">
+      <c r="AL16" s="36">
         <v>3</v>
       </c>
-      <c r="AM16" s="39">
+      <c r="AM16" s="38">
         <v>7</v>
       </c>
       <c r="AN16" s="10"/>
     </row>
     <row r="17" spans="1:40" s="12" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="64" t="s">
+      <c r="A17" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="52"/>
-      <c r="C17" s="52"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="112"/>
+      <c r="D17" s="119"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
-      <c r="S17" s="30" t="s">
+      <c r="S17" s="29" t="s">
         <v>17</v>
       </c>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="30"/>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="86"/>
-      <c r="AA17" s="86"/>
-      <c r="AB17" s="86"/>
-      <c r="AC17" s="51"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="78"/>
+      <c r="AA17" s="78"/>
+      <c r="AB17" s="78"/>
+      <c r="AC17" s="50"/>
       <c r="AD17" s="4"/>
       <c r="AE17" s="4"/>
-      <c r="AF17" s="30"/>
-      <c r="AG17" s="30"/>
-      <c r="AH17" s="30"/>
-      <c r="AI17" s="30"/>
-      <c r="AJ17" s="30"/>
-      <c r="AK17" s="30"/>
-      <c r="AL17" s="30"/>
-      <c r="AM17" s="30"/>
+      <c r="AF17" s="29"/>
+      <c r="AG17" s="29"/>
+      <c r="AH17" s="29"/>
+      <c r="AI17" s="29"/>
+      <c r="AJ17" s="29"/>
+      <c r="AK17" s="29"/>
+      <c r="AL17" s="29"/>
+      <c r="AM17" s="29"/>
       <c r="AN17" s="10"/>
     </row>
     <row r="18" spans="1:40" s="12" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="51"/>
-      <c r="H18" s="87" t="s">
+      <c r="B18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="50"/>
+      <c r="H18" s="120" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="88"/>
-      <c r="L18" s="89"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="51"/>
-      <c r="U18" s="51"/>
+      <c r="I18" s="120"/>
+      <c r="J18" s="120"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50"/>
       <c r="W18" s="4"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AB18" s="30" t="s">
+      <c r="X18" s="29"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="29"/>
+      <c r="AB18" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AH18" s="51"/>
-      <c r="AI18" s="51"/>
-      <c r="AJ18" s="51"/>
-      <c r="AK18" s="51"/>
-      <c r="AL18" s="51"/>
-      <c r="AM18" s="51"/>
+      <c r="AH18" s="50"/>
+      <c r="AI18" s="50"/>
+      <c r="AJ18" s="50"/>
+      <c r="AK18" s="50"/>
+      <c r="AL18" s="50"/>
+      <c r="AM18" s="50"/>
       <c r="AN18" s="10"/>
     </row>
     <row r="19" spans="1:40" s="12" customFormat="1" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="91"/>
-      <c r="C19" s="91"/>
-      <c r="D19" s="92"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="30" t="s">
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="122"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="30"/>
+      <c r="H19" s="29"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="51"/>
-      <c r="AF19" s="51"/>
-      <c r="AG19" s="51"/>
-      <c r="AH19" s="51"/>
-      <c r="AI19" s="51"/>
-      <c r="AJ19" s="51"/>
-      <c r="AK19" s="51"/>
-      <c r="AL19" s="51"/>
-      <c r="AM19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="50"/>
+      <c r="AD19" s="50"/>
+      <c r="AE19" s="50"/>
+      <c r="AF19" s="50"/>
+      <c r="AG19" s="50"/>
+      <c r="AH19" s="50"/>
+      <c r="AI19" s="50"/>
+      <c r="AJ19" s="50"/>
+      <c r="AK19" s="50"/>
+      <c r="AL19" s="50"/>
+      <c r="AM19" s="50"/>
       <c r="AN19" s="10"/>
     </row>
     <row r="20" spans="1:40" s="12" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="94"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
-      <c r="E20" s="35">
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="34">
         <v>0</v>
       </c>
-      <c r="F20" s="77">
+      <c r="F20" s="70">
         <v>1</v>
       </c>
-      <c r="G20" s="33">
+      <c r="G20" s="32">
         <v>0</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="29" t="s">
         <v>24</v>
       </c>
       <c r="J20" s="6"/>
-      <c r="M20" s="35">
+      <c r="M20" s="34">
         <v>1</v>
       </c>
-      <c r="N20" s="33">
+      <c r="N20" s="32">
         <v>1</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
-      <c r="R20" s="30" t="s">
+      <c r="R20" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="30"/>
-      <c r="W20" s="30"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="51"/>
-      <c r="Z20" s="51"/>
-      <c r="AA20" s="51"/>
-      <c r="AB20" s="51"/>
-      <c r="AC20" s="51"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="51"/>
-      <c r="AF20" s="51"/>
-      <c r="AG20" s="51"/>
-      <c r="AH20" s="51"/>
-      <c r="AI20" s="51"/>
-      <c r="AJ20" s="54"/>
-      <c r="AK20" s="51"/>
-      <c r="AL20" s="51"/>
-      <c r="AM20" s="51"/>
-      <c r="AN20" s="43"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="29"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="50"/>
+      <c r="AD20" s="50"/>
+      <c r="AE20" s="50"/>
+      <c r="AF20" s="50"/>
+      <c r="AG20" s="50"/>
+      <c r="AH20" s="50"/>
+      <c r="AI20" s="50"/>
+      <c r="AJ20" s="51"/>
+      <c r="AK20" s="50"/>
+      <c r="AL20" s="50"/>
+      <c r="AM20" s="50"/>
+      <c r="AN20" s="42"/>
     </row>
     <row r="21" spans="1:40" s="12" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="N21" s="54"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51"/>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
@@ -2470,465 +2450,453 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
-      <c r="AB21" s="30"/>
-      <c r="AC21" s="30"/>
-      <c r="AD21" s="30"/>
-      <c r="AE21" s="30"/>
-      <c r="AF21" s="30"/>
-      <c r="AG21" s="30"/>
-      <c r="AH21" s="30"/>
-      <c r="AI21" s="30"/>
-      <c r="AJ21" s="30"/>
-      <c r="AK21" s="30"/>
-      <c r="AL21" s="30"/>
-      <c r="AM21" s="30"/>
-      <c r="AN21" s="43"/>
+      <c r="AB21" s="29"/>
+      <c r="AC21" s="29"/>
+      <c r="AD21" s="29"/>
+      <c r="AE21" s="29"/>
+      <c r="AF21" s="29"/>
+      <c r="AG21" s="29"/>
+      <c r="AH21" s="29"/>
+      <c r="AI21" s="29"/>
+      <c r="AJ21" s="29"/>
+      <c r="AK21" s="29"/>
+      <c r="AL21" s="29"/>
+      <c r="AM21" s="29"/>
+      <c r="AN21" s="42"/>
     </row>
     <row r="22" spans="1:40" s="12" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="96"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="96"/>
-      <c r="J22" s="96"/>
-      <c r="K22" s="96"/>
-      <c r="L22" s="96"/>
-      <c r="M22" s="96"/>
-      <c r="N22" s="96"/>
-      <c r="O22" s="96"/>
-      <c r="P22" s="96"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="96"/>
-      <c r="S22" s="96"/>
-      <c r="T22" s="96"/>
-      <c r="U22" s="96"/>
-      <c r="V22" s="96"/>
-      <c r="W22" s="96"/>
-      <c r="X22" s="96"/>
-      <c r="Y22" s="96"/>
-      <c r="Z22" s="96"/>
-      <c r="AA22" s="96"/>
-      <c r="AB22" s="96"/>
-      <c r="AC22" s="96"/>
-      <c r="AD22" s="96"/>
-      <c r="AE22" s="96"/>
-      <c r="AF22" s="96"/>
-      <c r="AG22" s="96"/>
-      <c r="AH22" s="96"/>
-      <c r="AI22" s="96"/>
-      <c r="AJ22" s="96"/>
-      <c r="AK22" s="96"/>
-      <c r="AL22" s="96"/>
-      <c r="AM22" s="96"/>
-      <c r="AN22" s="97"/>
+      <c r="A22" s="82"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="83"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="83"/>
+      <c r="F22" s="83"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="83"/>
+      <c r="N22" s="83"/>
+      <c r="O22" s="83"/>
+      <c r="P22" s="83"/>
+      <c r="Q22" s="83"/>
+      <c r="R22" s="83"/>
+      <c r="S22" s="83"/>
+      <c r="T22" s="83"/>
+      <c r="U22" s="83"/>
+      <c r="V22" s="83"/>
+      <c r="W22" s="83"/>
+      <c r="X22" s="83"/>
+      <c r="Y22" s="83"/>
+      <c r="Z22" s="83"/>
+      <c r="AA22" s="83"/>
+      <c r="AB22" s="83"/>
+      <c r="AC22" s="83"/>
+      <c r="AD22" s="83"/>
+      <c r="AE22" s="83"/>
+      <c r="AF22" s="83"/>
+      <c r="AG22" s="83"/>
+      <c r="AH22" s="83"/>
+      <c r="AI22" s="83"/>
+      <c r="AJ22" s="83"/>
+      <c r="AK22" s="83"/>
+      <c r="AL22" s="83"/>
+      <c r="AM22" s="83"/>
+      <c r="AN22" s="84"/>
     </row>
     <row r="23" spans="1:40" s="12" customFormat="1" ht="6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="71"/>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="71"/>
-      <c r="H23" s="71"/>
-      <c r="I23" s="71"/>
-      <c r="J23" s="71"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="71"/>
-      <c r="M23" s="71"/>
-      <c r="N23" s="71"/>
-      <c r="O23" s="71"/>
-      <c r="P23" s="71"/>
-      <c r="Q23" s="71"/>
-      <c r="R23" s="71"/>
-      <c r="S23" s="71"/>
-      <c r="T23" s="71"/>
-      <c r="U23" s="71"/>
+      <c r="A23" s="64"/>
+      <c r="B23" s="64"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="64"/>
+      <c r="R23" s="64"/>
+      <c r="S23" s="64"/>
+      <c r="T23" s="64"/>
+      <c r="U23" s="64"/>
     </row>
     <row r="24" spans="1:40" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="98"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="66" t="s">
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="124"/>
+      <c r="E24" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="100"/>
-      <c r="G24" s="30"/>
-      <c r="I24" s="30" t="s">
+      <c r="F24" s="126"/>
+      <c r="G24" s="29"/>
+      <c r="I24" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="M24" s="68" t="s">
+      <c r="M24" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="N24" s="69" t="s">
+      <c r="N24" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="O24" s="69" t="s">
+      <c r="O24" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="P24" s="70"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="30" t="s">
+      <c r="P24" s="63"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="X24" s="73">
-        <v>7</v>
-      </c>
-      <c r="Y24" s="73">
-        <v>3</v>
-      </c>
-      <c r="Z24" s="73">
-        <v>5</v>
-      </c>
-      <c r="AA24" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB24" s="73">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="73">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="73"/>
-      <c r="AE24" s="74"/>
-      <c r="AF24" s="74"/>
-      <c r="AG24" s="74"/>
-      <c r="AH24" s="74"/>
-      <c r="AI24" s="74"/>
-      <c r="AJ24" s="74"/>
-      <c r="AK24" s="75"/>
-      <c r="AL24" s="75"/>
-      <c r="AM24" s="101"/>
+      <c r="X24" s="66"/>
+      <c r="Y24" s="66"/>
+      <c r="Z24" s="66"/>
+      <c r="AA24" s="66"/>
+      <c r="AB24" s="66"/>
+      <c r="AC24" s="66"/>
+      <c r="AD24" s="66"/>
+      <c r="AE24" s="67"/>
+      <c r="AF24" s="67"/>
+      <c r="AG24" s="67"/>
+      <c r="AH24" s="67"/>
+      <c r="AI24" s="67"/>
+      <c r="AJ24" s="67"/>
+      <c r="AK24" s="68"/>
+      <c r="AL24" s="68"/>
+      <c r="AM24" s="85"/>
       <c r="AN24" s="10"/>
     </row>
     <row r="25" spans="1:40" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="64" t="s">
+      <c r="A25" s="111" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="52"/>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="102" t="s">
+      <c r="B25" s="112"/>
+      <c r="C25" s="112"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="103" t="s">
+      <c r="F25" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="103" t="s">
+      <c r="G25" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="H25" s="104"/>
-      <c r="I25" s="104"/>
-      <c r="J25" s="104"/>
-      <c r="K25" s="104"/>
-      <c r="L25" s="104"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="104"/>
-      <c r="O25" s="104"/>
-      <c r="P25" s="105"/>
-      <c r="Q25" s="71"/>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
-      <c r="AA25" s="30"/>
-      <c r="AB25" s="30"/>
-      <c r="AC25" s="30"/>
-      <c r="AD25" s="30"/>
-      <c r="AE25" s="30"/>
-      <c r="AF25" s="30"/>
-      <c r="AG25" s="30"/>
-      <c r="AH25" s="30"/>
-      <c r="AI25" s="30"/>
-      <c r="AJ25" s="30"/>
-      <c r="AK25" s="30"/>
-      <c r="AL25" s="30"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="88"/>
+      <c r="O25" s="88"/>
+      <c r="P25" s="89"/>
+      <c r="Q25" s="64"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="29"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
+      <c r="Z25" s="29"/>
+      <c r="AA25" s="29"/>
+      <c r="AB25" s="29"/>
+      <c r="AC25" s="29"/>
+      <c r="AD25" s="29"/>
+      <c r="AE25" s="29"/>
+      <c r="AF25" s="29"/>
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="29"/>
+      <c r="AI25" s="29"/>
+      <c r="AJ25" s="29"/>
+      <c r="AK25" s="29"/>
+      <c r="AL25" s="29"/>
       <c r="AM25" s="6"/>
       <c r="AN25" s="10"/>
     </row>
     <row r="26" spans="1:40" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="52"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="52"/>
-      <c r="E26" s="81">
+      <c r="B26" s="112"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="112"/>
+      <c r="E26" s="74">
         <v>1</v>
       </c>
-      <c r="F26" s="82">
+      <c r="F26" s="75">
         <v>4</v>
       </c>
-      <c r="G26" s="82">
+      <c r="G26" s="75">
         <v>0</v>
       </c>
-      <c r="H26" s="82">
+      <c r="H26" s="75">
         <v>1</v>
       </c>
-      <c r="I26" s="83">
+      <c r="I26" s="76">
         <v>7</v>
       </c>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="30"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
       <c r="N26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="30" t="s">
+      <c r="S26" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="W26" s="30"/>
-      <c r="Z26" s="36" t="s">
+      <c r="W26" s="29"/>
+      <c r="Z26" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="AA26" s="37">
+      <c r="AA26" s="36">
         <v>7</v>
       </c>
-      <c r="AB26" s="39">
+      <c r="AB26" s="38">
         <v>9</v>
       </c>
-      <c r="AC26" s="84" t="s">
+      <c r="AC26" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="AD26" s="36">
+      <c r="AD26" s="35">
         <v>7</v>
       </c>
-      <c r="AE26" s="37">
+      <c r="AE26" s="36">
         <v>8</v>
       </c>
-      <c r="AF26" s="39">
+      <c r="AF26" s="38">
         <v>9</v>
       </c>
-      <c r="AG26" s="84" t="s">
+      <c r="AG26" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="AH26" s="36">
+      <c r="AH26" s="35">
         <v>1</v>
       </c>
-      <c r="AI26" s="37">
+      <c r="AI26" s="36">
         <v>1</v>
       </c>
-      <c r="AJ26" s="37">
+      <c r="AJ26" s="36">
         <v>1</v>
       </c>
-      <c r="AK26" s="37">
+      <c r="AK26" s="36">
         <v>1</v>
       </c>
-      <c r="AL26" s="37">
+      <c r="AL26" s="36">
         <v>1</v>
       </c>
-      <c r="AM26" s="39">
+      <c r="AM26" s="38">
         <v>1</v>
       </c>
       <c r="AN26" s="10"/>
     </row>
     <row r="27" spans="1:40" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="111" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="53"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
-      <c r="S27" s="30" t="s">
+      <c r="S27" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="W27" s="30"/>
-      <c r="X27" s="30"/>
-      <c r="Y27" s="30"/>
-      <c r="Z27" s="86"/>
-      <c r="AA27" s="86"/>
-      <c r="AB27" s="86"/>
-      <c r="AC27" s="51"/>
-      <c r="AF27" s="30"/>
-      <c r="AG27" s="30"/>
-      <c r="AH27" s="30"/>
-      <c r="AI27" s="30"/>
-      <c r="AJ27" s="30"/>
-      <c r="AK27" s="30"/>
-      <c r="AL27" s="30"/>
-      <c r="AM27" s="30"/>
+      <c r="W27" s="29"/>
+      <c r="X27" s="29"/>
+      <c r="Y27" s="29"/>
+      <c r="Z27" s="78"/>
+      <c r="AA27" s="78"/>
+      <c r="AB27" s="78"/>
+      <c r="AC27" s="50"/>
+      <c r="AF27" s="29"/>
+      <c r="AG27" s="29"/>
+      <c r="AH27" s="29"/>
+      <c r="AI27" s="29"/>
+      <c r="AJ27" s="29"/>
+      <c r="AK27" s="29"/>
+      <c r="AL27" s="29"/>
+      <c r="AM27" s="29"/>
       <c r="AN27" s="10"/>
     </row>
     <row r="28" spans="1:40" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="51"/>
-      <c r="H28" s="106" t="s">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="50"/>
+      <c r="H28" s="114" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="107"/>
-      <c r="J28" s="107"/>
-      <c r="K28" s="108"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="X28" s="30"/>
-      <c r="Y28" s="30"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="116"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="X28" s="29"/>
+      <c r="Y28" s="29"/>
       <c r="AA28" s="6"/>
-      <c r="AB28" s="30" t="s">
+      <c r="AB28" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
+      <c r="AH28" s="50"/>
+      <c r="AI28" s="50"/>
+      <c r="AJ28" s="50"/>
+      <c r="AK28" s="50"/>
+      <c r="AL28" s="50"/>
+      <c r="AM28" s="50"/>
       <c r="AN28" s="10"/>
     </row>
     <row r="29" spans="1:40" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="B29" s="91"/>
-      <c r="C29" s="91"/>
-      <c r="D29" s="91"/>
-      <c r="E29" s="93"/>
-      <c r="F29" s="30" t="s">
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
+      <c r="E29" s="80"/>
+      <c r="F29" s="29" t="s">
         <v>22</v>
       </c>
       <c r="I29" s="6"/>
-      <c r="J29" s="109"/>
-      <c r="K29" s="109"/>
-      <c r="L29" s="109"/>
-      <c r="M29" s="109"/>
-      <c r="N29" s="109"/>
-      <c r="O29" s="109"/>
-      <c r="P29" s="109"/>
-      <c r="Q29" s="109"/>
-      <c r="R29" s="109"/>
-      <c r="S29" s="109"/>
-      <c r="T29" s="109"/>
-      <c r="U29" s="109"/>
-      <c r="V29" s="109"/>
-      <c r="W29" s="109"/>
-      <c r="X29" s="109"/>
-      <c r="Y29" s="110"/>
-      <c r="Z29" s="109"/>
-      <c r="AA29" s="109"/>
-      <c r="AB29" s="109"/>
-      <c r="AC29" s="109"/>
-      <c r="AD29" s="109"/>
-      <c r="AE29" s="109"/>
-      <c r="AF29" s="109"/>
-      <c r="AG29" s="109"/>
-      <c r="AH29" s="109"/>
-      <c r="AI29" s="109"/>
-      <c r="AJ29" s="109"/>
-      <c r="AK29" s="109"/>
-      <c r="AL29" s="109"/>
-      <c r="AM29" s="109"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="90"/>
+      <c r="Q29" s="90"/>
+      <c r="R29" s="90"/>
+      <c r="S29" s="90"/>
+      <c r="T29" s="90"/>
+      <c r="U29" s="90"/>
+      <c r="V29" s="90"/>
+      <c r="W29" s="90"/>
+      <c r="X29" s="90"/>
+      <c r="Y29" s="91"/>
+      <c r="Z29" s="90"/>
+      <c r="AA29" s="90"/>
+      <c r="AB29" s="90"/>
+      <c r="AC29" s="90"/>
+      <c r="AD29" s="90"/>
+      <c r="AE29" s="90"/>
+      <c r="AF29" s="90"/>
+      <c r="AG29" s="90"/>
+      <c r="AH29" s="90"/>
+      <c r="AI29" s="90"/>
+      <c r="AJ29" s="90"/>
+      <c r="AK29" s="90"/>
+      <c r="AL29" s="90"/>
+      <c r="AM29" s="90"/>
       <c r="AN29" s="10"/>
     </row>
     <row r="30" spans="1:40" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="50" t="s">
+      <c r="A30" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
-      <c r="E30" s="35">
+      <c r="B30" s="81"/>
+      <c r="C30" s="81"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="34">
         <v>0</v>
       </c>
-      <c r="F30" s="77">
+      <c r="F30" s="70">
         <v>1</v>
       </c>
-      <c r="G30" s="33">
+      <c r="G30" s="32">
         <v>0</v>
       </c>
-      <c r="I30" s="30" t="s">
+      <c r="I30" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="M30" s="35">
+      <c r="M30" s="34">
         <v>1</v>
       </c>
-      <c r="N30" s="33">
+      <c r="N30" s="32">
         <v>1</v>
       </c>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
-      <c r="R30" s="30" t="s">
+      <c r="R30" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
-      <c r="U30" s="30"/>
-      <c r="V30" s="30"/>
-      <c r="W30" s="30"/>
-      <c r="X30" s="51"/>
-      <c r="Y30" s="51"/>
-      <c r="Z30" s="51"/>
-      <c r="AA30" s="51"/>
-      <c r="AB30" s="51"/>
-      <c r="AC30" s="51"/>
-      <c r="AD30" s="51"/>
-      <c r="AE30" s="51"/>
-      <c r="AF30" s="51"/>
-      <c r="AG30" s="51"/>
-      <c r="AH30" s="51"/>
-      <c r="AI30" s="51"/>
-      <c r="AJ30" s="54"/>
-      <c r="AK30" s="51"/>
-      <c r="AL30" s="51"/>
-      <c r="AM30" s="51"/>
-      <c r="AN30" s="43"/>
+      <c r="S30" s="29"/>
+      <c r="T30" s="29"/>
+      <c r="U30" s="29"/>
+      <c r="V30" s="29"/>
+      <c r="W30" s="29"/>
+      <c r="X30" s="50"/>
+      <c r="Y30" s="50"/>
+      <c r="Z30" s="50"/>
+      <c r="AA30" s="50"/>
+      <c r="AB30" s="50"/>
+      <c r="AC30" s="50"/>
+      <c r="AD30" s="50"/>
+      <c r="AE30" s="50"/>
+      <c r="AF30" s="50"/>
+      <c r="AG30" s="50"/>
+      <c r="AH30" s="50"/>
+      <c r="AI30" s="50"/>
+      <c r="AJ30" s="51"/>
+      <c r="AK30" s="50"/>
+      <c r="AL30" s="50"/>
+      <c r="AM30" s="50"/>
+      <c r="AN30" s="42"/>
     </row>
     <row r="31" spans="1:40" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="50" t="s">
+      <c r="A31" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="94"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="54"/>
-      <c r="H31" s="54"/>
-      <c r="I31" s="54"/>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="54"/>
-      <c r="N31" s="54"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="51"/>
+      <c r="M31" s="51"/>
+      <c r="N31" s="51"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
@@ -2942,313 +2910,313 @@
       <c r="Y31" s="6"/>
       <c r="Z31" s="6"/>
       <c r="AA31" s="6"/>
-      <c r="AB31" s="30"/>
-      <c r="AC31" s="30"/>
-      <c r="AD31" s="30"/>
-      <c r="AE31" s="30"/>
-      <c r="AF31" s="30"/>
-      <c r="AG31" s="30"/>
-      <c r="AH31" s="30"/>
-      <c r="AI31" s="30"/>
-      <c r="AJ31" s="30"/>
-      <c r="AK31" s="30"/>
-      <c r="AL31" s="30"/>
-      <c r="AM31" s="30"/>
-      <c r="AN31" s="43"/>
+      <c r="AB31" s="29"/>
+      <c r="AC31" s="29"/>
+      <c r="AD31" s="29"/>
+      <c r="AE31" s="29"/>
+      <c r="AF31" s="29"/>
+      <c r="AG31" s="29"/>
+      <c r="AH31" s="29"/>
+      <c r="AI31" s="29"/>
+      <c r="AJ31" s="29"/>
+      <c r="AK31" s="29"/>
+      <c r="AL31" s="29"/>
+      <c r="AM31" s="29"/>
+      <c r="AN31" s="42"/>
     </row>
     <row r="32" spans="1:40" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="50"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="30"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
-      <c r="M32" s="30"/>
-      <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="30"/>
-      <c r="Q32" s="30"/>
-      <c r="R32" s="30"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
-      <c r="U32" s="30"/>
-      <c r="V32" s="30"/>
-      <c r="W32" s="30"/>
-      <c r="X32" s="30"/>
-      <c r="Y32" s="30"/>
-      <c r="Z32" s="30"/>
-      <c r="AA32" s="30"/>
-      <c r="AB32" s="30"/>
-      <c r="AC32" s="30"/>
-      <c r="AD32" s="30"/>
-      <c r="AE32" s="30"/>
-      <c r="AF32" s="30"/>
-      <c r="AG32" s="30"/>
-      <c r="AH32" s="30"/>
-      <c r="AI32" s="30"/>
-      <c r="AJ32" s="30"/>
-      <c r="AK32" s="30"/>
-      <c r="AL32" s="30"/>
-      <c r="AM32" s="30"/>
-      <c r="AN32" s="43"/>
+      <c r="A32" s="49"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="29"/>
+      <c r="U32" s="29"/>
+      <c r="V32" s="29"/>
+      <c r="W32" s="29"/>
+      <c r="X32" s="29"/>
+      <c r="Y32" s="29"/>
+      <c r="Z32" s="29"/>
+      <c r="AA32" s="29"/>
+      <c r="AB32" s="29"/>
+      <c r="AC32" s="29"/>
+      <c r="AD32" s="29"/>
+      <c r="AE32" s="29"/>
+      <c r="AF32" s="29"/>
+      <c r="AG32" s="29"/>
+      <c r="AH32" s="29"/>
+      <c r="AI32" s="29"/>
+      <c r="AJ32" s="29"/>
+      <c r="AK32" s="29"/>
+      <c r="AL32" s="29"/>
+      <c r="AM32" s="29"/>
+      <c r="AN32" s="42"/>
     </row>
     <row r="33" spans="1:40" ht="3.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="111"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="59"/>
-      <c r="N33" s="59"/>
-      <c r="O33" s="59"/>
-      <c r="P33" s="59"/>
-      <c r="Q33" s="59"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="59"/>
-      <c r="T33" s="59"/>
-      <c r="U33" s="59"/>
-      <c r="V33" s="59"/>
-      <c r="W33" s="59"/>
-      <c r="X33" s="59"/>
-      <c r="Y33" s="59"/>
-      <c r="Z33" s="59"/>
-      <c r="AA33" s="59"/>
-      <c r="AB33" s="59"/>
-      <c r="AC33" s="59"/>
-      <c r="AD33" s="59"/>
-      <c r="AE33" s="59"/>
-      <c r="AF33" s="59"/>
-      <c r="AG33" s="59"/>
-      <c r="AH33" s="59"/>
-      <c r="AI33" s="59"/>
-      <c r="AJ33" s="59"/>
-      <c r="AK33" s="59"/>
-      <c r="AL33" s="59"/>
-      <c r="AM33" s="59"/>
-      <c r="AN33" s="62"/>
+      <c r="A33" s="92"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
+      <c r="J33" s="56"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="56"/>
+      <c r="M33" s="56"/>
+      <c r="N33" s="56"/>
+      <c r="O33" s="56"/>
+      <c r="P33" s="56"/>
+      <c r="Q33" s="56"/>
+      <c r="R33" s="56"/>
+      <c r="S33" s="56"/>
+      <c r="T33" s="56"/>
+      <c r="U33" s="56"/>
+      <c r="V33" s="56"/>
+      <c r="W33" s="56"/>
+      <c r="X33" s="56"/>
+      <c r="Y33" s="56"/>
+      <c r="Z33" s="56"/>
+      <c r="AA33" s="56"/>
+      <c r="AB33" s="56"/>
+      <c r="AC33" s="56"/>
+      <c r="AD33" s="56"/>
+      <c r="AE33" s="56"/>
+      <c r="AF33" s="56"/>
+      <c r="AG33" s="56"/>
+      <c r="AH33" s="56"/>
+      <c r="AI33" s="56"/>
+      <c r="AJ33" s="56"/>
+      <c r="AK33" s="56"/>
+      <c r="AL33" s="56"/>
+      <c r="AM33" s="56"/>
+      <c r="AN33" s="59"/>
     </row>
     <row r="34" spans="1:40" s="12" customFormat="1" ht="3" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="112"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
-      <c r="M34" s="30"/>
-      <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="30"/>
-      <c r="Q34" s="30"/>
-      <c r="R34" s="30"/>
-      <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
-      <c r="U34" s="30"/>
-      <c r="V34" s="30"/>
-      <c r="W34" s="30"/>
-      <c r="X34" s="30"/>
-      <c r="Y34" s="30"/>
-      <c r="Z34" s="30"/>
-      <c r="AA34" s="30"/>
-      <c r="AB34" s="30"/>
-      <c r="AC34" s="30"/>
-      <c r="AD34" s="30"/>
-      <c r="AE34" s="30"/>
-      <c r="AF34" s="30"/>
-      <c r="AG34" s="30"/>
-      <c r="AH34" s="30"/>
-      <c r="AI34" s="30"/>
-      <c r="AJ34" s="30"/>
-      <c r="AK34" s="30"/>
-      <c r="AL34" s="30"/>
-      <c r="AM34" s="30"/>
-      <c r="AN34" s="43"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="29"/>
+      <c r="V34" s="29"/>
+      <c r="W34" s="29"/>
+      <c r="X34" s="29"/>
+      <c r="Y34" s="29"/>
+      <c r="Z34" s="29"/>
+      <c r="AA34" s="29"/>
+      <c r="AB34" s="29"/>
+      <c r="AC34" s="29"/>
+      <c r="AD34" s="29"/>
+      <c r="AE34" s="29"/>
+      <c r="AF34" s="29"/>
+      <c r="AG34" s="29"/>
+      <c r="AH34" s="29"/>
+      <c r="AI34" s="29"/>
+      <c r="AJ34" s="29"/>
+      <c r="AK34" s="29"/>
+      <c r="AL34" s="29"/>
+      <c r="AM34" s="29"/>
+      <c r="AN34" s="42"/>
     </row>
     <row r="35" spans="1:40" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="113"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="113"/>
-      <c r="L35" s="113"/>
-      <c r="M35" s="113"/>
-      <c r="N35" s="113"/>
-      <c r="O35" s="113"/>
-      <c r="P35" s="114" t="s">
+      <c r="A35" s="94"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="Q35" s="115"/>
-      <c r="R35" s="115"/>
-      <c r="S35" s="115"/>
-      <c r="T35" s="115"/>
-      <c r="U35" s="116"/>
-      <c r="V35" s="116"/>
-      <c r="W35" s="116"/>
-      <c r="X35" s="117"/>
-      <c r="Y35" s="115" t="s">
+      <c r="Q35" s="96"/>
+      <c r="R35" s="96"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="96"/>
+      <c r="U35" s="97"/>
+      <c r="V35" s="97"/>
+      <c r="W35" s="97"/>
+      <c r="X35" s="98"/>
+      <c r="Y35" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="Z35" s="115"/>
-      <c r="AA35" s="116"/>
-      <c r="AB35" s="115"/>
-      <c r="AC35" s="117"/>
-      <c r="AD35" s="115" t="s">
+      <c r="Z35" s="96"/>
+      <c r="AA35" s="97"/>
+      <c r="AB35" s="96"/>
+      <c r="AC35" s="98"/>
+      <c r="AD35" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="AE35" s="115"/>
-      <c r="AF35" s="116"/>
-      <c r="AG35" s="115"/>
-      <c r="AH35" s="117"/>
-      <c r="AI35" s="114" t="s">
+      <c r="AE35" s="96"/>
+      <c r="AF35" s="97"/>
+      <c r="AG35" s="96"/>
+      <c r="AH35" s="98"/>
+      <c r="AI35" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="AJ35" s="115"/>
-      <c r="AK35" s="115"/>
-      <c r="AL35" s="115"/>
-      <c r="AM35" s="117"/>
+      <c r="AJ35" s="96"/>
+      <c r="AK35" s="96"/>
+      <c r="AL35" s="96"/>
+      <c r="AM35" s="98"/>
     </row>
     <row r="36" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="113"/>
-      <c r="B36" s="113"/>
-      <c r="C36" s="113"/>
-      <c r="D36" s="113"/>
-      <c r="E36" s="113"/>
-      <c r="F36" s="113"/>
-      <c r="G36" s="113"/>
-      <c r="H36" s="113"/>
-      <c r="I36" s="113"/>
-      <c r="J36" s="113"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="113"/>
-      <c r="M36" s="113"/>
-      <c r="N36" s="113"/>
-      <c r="O36" s="113"/>
-      <c r="P36" s="118"/>
-      <c r="Q36" s="119"/>
-      <c r="R36" s="119"/>
-      <c r="S36" s="119"/>
-      <c r="T36" s="119"/>
+      <c r="A36" s="94"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="94"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="94"/>
+      <c r="H36" s="94"/>
+      <c r="I36" s="94"/>
+      <c r="J36" s="94"/>
+      <c r="K36" s="94"/>
+      <c r="L36" s="94"/>
+      <c r="M36" s="94"/>
+      <c r="N36" s="94"/>
+      <c r="O36" s="94"/>
+      <c r="P36" s="99"/>
+      <c r="Q36" s="100"/>
+      <c r="R36" s="100"/>
+      <c r="S36" s="100"/>
+      <c r="T36" s="100"/>
       <c r="U36" s="6"/>
       <c r="V36" s="6"/>
       <c r="W36" s="6"/>
-      <c r="X36" s="120"/>
-      <c r="Y36" s="121"/>
-      <c r="Z36" s="122"/>
-      <c r="AA36" s="122"/>
-      <c r="AB36" s="122"/>
-      <c r="AC36" s="123"/>
-      <c r="AD36" s="121"/>
-      <c r="AE36" s="122"/>
-      <c r="AF36" s="122"/>
-      <c r="AG36" s="122"/>
-      <c r="AH36" s="123"/>
-      <c r="AI36" s="121"/>
-      <c r="AJ36" s="122"/>
-      <c r="AK36" s="122"/>
-      <c r="AL36" s="122"/>
-      <c r="AM36" s="123"/>
+      <c r="X36" s="101"/>
+      <c r="Y36" s="102"/>
+      <c r="Z36" s="103"/>
+      <c r="AA36" s="103"/>
+      <c r="AB36" s="103"/>
+      <c r="AC36" s="104"/>
+      <c r="AD36" s="102"/>
+      <c r="AE36" s="103"/>
+      <c r="AF36" s="103"/>
+      <c r="AG36" s="103"/>
+      <c r="AH36" s="104"/>
+      <c r="AI36" s="102"/>
+      <c r="AJ36" s="103"/>
+      <c r="AK36" s="103"/>
+      <c r="AL36" s="103"/>
+      <c r="AM36" s="104"/>
     </row>
     <row r="37" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="113"/>
-      <c r="B37" s="113"/>
-      <c r="C37" s="113"/>
-      <c r="D37" s="113"/>
-      <c r="E37" s="113"/>
-      <c r="F37" s="113"/>
-      <c r="G37" s="113"/>
-      <c r="H37" s="113"/>
-      <c r="I37" s="113"/>
-      <c r="J37" s="113"/>
-      <c r="K37" s="113"/>
-      <c r="L37" s="113"/>
-      <c r="M37" s="113"/>
-      <c r="N37" s="113"/>
-      <c r="O37" s="113"/>
-      <c r="P37" s="118"/>
-      <c r="Q37" s="119"/>
-      <c r="R37" s="119"/>
-      <c r="S37" s="119"/>
-      <c r="T37" s="119"/>
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="94"/>
+      <c r="L37" s="94"/>
+      <c r="M37" s="94"/>
+      <c r="N37" s="94"/>
+      <c r="O37" s="94"/>
+      <c r="P37" s="99"/>
+      <c r="Q37" s="100"/>
+      <c r="R37" s="100"/>
+      <c r="S37" s="100"/>
+      <c r="T37" s="100"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
       <c r="W37" s="6"/>
-      <c r="X37" s="120"/>
-      <c r="Y37" s="121"/>
-      <c r="Z37" s="122"/>
-      <c r="AA37" s="122"/>
-      <c r="AB37" s="122"/>
-      <c r="AC37" s="123"/>
-      <c r="AD37" s="121"/>
-      <c r="AE37" s="122"/>
-      <c r="AF37" s="122"/>
-      <c r="AG37" s="122"/>
-      <c r="AH37" s="123"/>
-      <c r="AI37" s="121"/>
-      <c r="AJ37" s="122"/>
-      <c r="AK37" s="122"/>
-      <c r="AL37" s="122"/>
-      <c r="AM37" s="123"/>
+      <c r="X37" s="101"/>
+      <c r="Y37" s="102"/>
+      <c r="Z37" s="103"/>
+      <c r="AA37" s="103"/>
+      <c r="AB37" s="103"/>
+      <c r="AC37" s="104"/>
+      <c r="AD37" s="102"/>
+      <c r="AE37" s="103"/>
+      <c r="AF37" s="103"/>
+      <c r="AG37" s="103"/>
+      <c r="AH37" s="104"/>
+      <c r="AI37" s="102"/>
+      <c r="AJ37" s="103"/>
+      <c r="AK37" s="103"/>
+      <c r="AL37" s="103"/>
+      <c r="AM37" s="104"/>
     </row>
     <row r="38" spans="1:40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="113"/>
-      <c r="P38" s="124"/>
-      <c r="Q38" s="125"/>
-      <c r="R38" s="125"/>
-      <c r="S38" s="125"/>
-      <c r="T38" s="125"/>
-      <c r="U38" s="25"/>
-      <c r="V38" s="25"/>
-      <c r="W38" s="25"/>
-      <c r="X38" s="126"/>
-      <c r="Y38" s="127"/>
-      <c r="Z38" s="128"/>
-      <c r="AA38" s="128"/>
-      <c r="AB38" s="128"/>
-      <c r="AC38" s="129"/>
-      <c r="AD38" s="127"/>
-      <c r="AE38" s="128"/>
-      <c r="AF38" s="128"/>
-      <c r="AG38" s="128"/>
-      <c r="AH38" s="129"/>
-      <c r="AI38" s="127"/>
-      <c r="AJ38" s="128"/>
-      <c r="AK38" s="128"/>
-      <c r="AL38" s="128"/>
-      <c r="AM38" s="129"/>
+      <c r="A38" s="94"/>
+      <c r="P38" s="105"/>
+      <c r="Q38" s="106"/>
+      <c r="R38" s="106"/>
+      <c r="S38" s="106"/>
+      <c r="T38" s="106"/>
+      <c r="U38" s="24"/>
+      <c r="V38" s="24"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="107"/>
+      <c r="Y38" s="108"/>
+      <c r="Z38" s="109"/>
+      <c r="AA38" s="109"/>
+      <c r="AB38" s="109"/>
+      <c r="AC38" s="110"/>
+      <c r="AD38" s="108"/>
+      <c r="AE38" s="109"/>
+      <c r="AF38" s="109"/>
+      <c r="AG38" s="109"/>
+      <c r="AH38" s="110"/>
+      <c r="AI38" s="108"/>
+      <c r="AJ38" s="109"/>
+      <c r="AK38" s="109"/>
+      <c r="AL38" s="109"/>
+      <c r="AM38" s="110"/>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A39" s="113"/>
+      <c r="A39" s="94"/>
       <c r="V39" s="6"/>
-      <c r="W39" s="30"/>
-      <c r="X39" s="30"/>
-      <c r="Y39" s="30"/>
-      <c r="Z39" s="30"/>
-      <c r="AA39" s="30"/>
-      <c r="AB39" s="30"/>
+      <c r="W39" s="29"/>
+      <c r="X39" s="29"/>
+      <c r="Y39" s="29"/>
+      <c r="Z39" s="29"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="29"/>
       <c r="AC39" s="6"/>
       <c r="AD39" s="6"/>
       <c r="AE39" s="6"/>
@@ -3264,23 +3232,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="H28:K28"/>
-    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="V5:AB5"/>
+    <mergeCell ref="AJ10:AL10"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="V5:AB5"/>
-    <mergeCell ref="AJ10:AL10"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="H28:K28"/>
+    <mergeCell ref="A29:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>